<commit_message>
commit of data file to allow merge
</commit_message>
<xml_diff>
--- a/data/embodied_emissions_envelope.xlsx
+++ b/data/embodied_emissions_envelope.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4176" windowHeight="3156"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4180" windowHeight="3160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="135">
   <si>
     <t>Abk</t>
   </si>
@@ -317,9 +317,6 @@
     <t>UBA_12</t>
   </si>
   <si>
-    <t>floor</t>
-  </si>
-  <si>
     <t>Stahlbeton</t>
   </si>
   <si>
@@ -372,6 +369,66 @@
   </si>
   <si>
     <t>UBA_KFW_40_wall_wood</t>
+  </si>
+  <si>
+    <t>N11_1</t>
+  </si>
+  <si>
+    <t>Flachs</t>
+  </si>
+  <si>
+    <t>N11_2</t>
+  </si>
+  <si>
+    <t>N11_wall_wood</t>
+  </si>
+  <si>
+    <t>N11_wall_concrete</t>
+  </si>
+  <si>
+    <t>N11_roof_wood</t>
+  </si>
+  <si>
+    <t>N11_roof_concrete</t>
+  </si>
+  <si>
+    <t>Beton Flachsdämmung</t>
+  </si>
+  <si>
+    <t>Holz100 Flachsdämmung</t>
+  </si>
+  <si>
+    <t>N11_3</t>
+  </si>
+  <si>
+    <t>N11_4</t>
+  </si>
+  <si>
+    <t>flachs</t>
+  </si>
+  <si>
+    <t>Beton Flachsdämmung Spanplatte PEDichtung</t>
+  </si>
+  <si>
+    <t>ceiling</t>
+  </si>
+  <si>
+    <t>N11_all_stb</t>
+  </si>
+  <si>
+    <t>N11_all_wood_concrete</t>
+  </si>
+  <si>
+    <t>Holzbeton und rammed earth</t>
+  </si>
+  <si>
+    <t>N11_5</t>
+  </si>
+  <si>
+    <t>N11_6</t>
+  </si>
+  <si>
+    <t>woodcrete</t>
   </si>
 </sst>
 </file>
@@ -478,7 +535,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -900,7 +956,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1018,7 +1073,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1122,7 +1176,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1218,7 +1271,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3250,13 +3302,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>445770</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>49530</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3280,13 +3332,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>11430</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3574,26 +3626,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="79.77734375" customWidth="1"/>
-    <col min="3" max="3" width="50.88671875" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="32.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="79.81640625" customWidth="1"/>
+    <col min="3" max="3" width="50.90625" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" customWidth="1"/>
+    <col min="6" max="6" width="32.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
     <col min="8" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="26.21875" customWidth="1"/>
-    <col min="11" max="11" width="15.21875" customWidth="1"/>
+    <col min="10" max="10" width="26.1796875" customWidth="1"/>
+    <col min="11" max="11" width="15.1796875" customWidth="1"/>
     <col min="12" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -3637,7 +3690,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3682,7 +3735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -3727,7 +3780,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3772,7 +3825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -3817,7 +3870,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3862,7 +3915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -3907,7 +3960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3952,7 +4005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -3997,7 +4050,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -4042,7 +4095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -4087,7 +4140,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -4132,7 +4185,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -4177,7 +4230,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -4222,7 +4275,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -4267,7 +4320,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -4312,7 +4365,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -4357,12 +4410,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="M18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -4394,7 +4447,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -4426,7 +4479,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -4464,7 +4517,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -4502,7 +4555,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -4540,7 +4593,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -4578,7 +4631,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -4616,12 +4669,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
         <v>92</v>
@@ -4654,74 +4707,39 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28">
-        <v>0.16</v>
-      </c>
-      <c r="F28" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28">
-        <v>0.19</v>
-      </c>
-      <c r="H28">
-        <v>71</v>
-      </c>
-      <c r="I28">
-        <v>196</v>
-      </c>
-      <c r="K28" t="s">
-        <v>7</v>
-      </c>
-      <c r="M28">
-        <v>60</v>
-      </c>
-      <c r="N28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="E29">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="G29">
         <v>0.13</v>
       </c>
       <c r="H29">
-        <v>74</v>
+        <v>-276</v>
       </c>
       <c r="I29">
-        <v>225</v>
+        <v>173</v>
+      </c>
+      <c r="J29">
+        <v>193</v>
       </c>
       <c r="K29" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="M29">
         <v>60</v>
@@ -4730,33 +4748,36 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="E30">
         <v>0.28000000000000003</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="G30">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="H30">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="I30">
-        <v>239</v>
+        <v>67</v>
+      </c>
+      <c r="J30">
+        <v>535</v>
       </c>
       <c r="K30" t="s">
         <v>7</v>
@@ -4768,112 +4789,36 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31">
-        <v>0.15</v>
-      </c>
-      <c r="F31" t="s">
-        <v>109</v>
-      </c>
-      <c r="G31">
-        <v>0.25</v>
-      </c>
-      <c r="H31">
-        <v>-22</v>
-      </c>
-      <c r="I31">
-        <v>68</v>
-      </c>
-      <c r="K31" t="s">
-        <v>17</v>
-      </c>
-      <c r="M31">
-        <v>60</v>
-      </c>
-      <c r="N31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" t="s">
-        <v>105</v>
-      </c>
-      <c r="E32">
-        <v>0.3</v>
-      </c>
-      <c r="F32" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H32">
-        <v>-26</v>
-      </c>
-      <c r="I32">
-        <v>87</v>
-      </c>
-      <c r="K32" t="s">
-        <v>17</v>
-      </c>
-      <c r="M32">
-        <v>60</v>
-      </c>
-      <c r="N32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="E33">
-        <v>0.32</v>
+        <v>0.16</v>
       </c>
       <c r="F33" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="G33">
-        <v>0.12</v>
+        <v>0.19</v>
       </c>
       <c r="H33">
-        <v>-27</v>
+        <v>71</v>
       </c>
       <c r="I33">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="K33" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="M33">
         <v>60</v>
@@ -4882,71 +4827,147 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34">
+        <v>0.24</v>
+      </c>
+      <c r="F34" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34">
+        <v>0.13</v>
+      </c>
+      <c r="H34">
+        <v>74</v>
+      </c>
+      <c r="I34">
+        <v>225</v>
+      </c>
+      <c r="K34" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34">
+        <v>60</v>
+      </c>
+      <c r="N34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35">
+        <v>0.11</v>
+      </c>
+      <c r="H35">
+        <v>76</v>
+      </c>
+      <c r="I35">
+        <v>239</v>
+      </c>
+      <c r="K35" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35">
+        <v>60</v>
+      </c>
+      <c r="N35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D36" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F36" t="s">
-        <v>99</v>
-      </c>
-      <c r="G36" t="s">
-        <v>99</v>
+        <v>108</v>
+      </c>
+      <c r="G36">
+        <v>0.25</v>
       </c>
       <c r="H36">
-        <v>58</v>
+        <v>-22</v>
       </c>
       <c r="I36">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="K36" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="M36">
         <v>60</v>
       </c>
       <c r="N36" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D37" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37">
+        <v>0.3</v>
+      </c>
+      <c r="F37" t="s">
         <v>108</v>
       </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>99</v>
-      </c>
-      <c r="G37" t="s">
-        <v>99</v>
+      <c r="G37">
+        <v>0.14000000000000001</v>
       </c>
       <c r="H37">
-        <v>-55</v>
+        <v>-26</v>
       </c>
       <c r="I37">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="K37" t="s">
         <v>17</v>
@@ -4955,202 +4976,477 @@
         <v>60</v>
       </c>
       <c r="N37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38">
+        <v>0.32</v>
+      </c>
+      <c r="F38" t="s">
+        <v>108</v>
+      </c>
+      <c r="G38">
+        <v>0.12</v>
+      </c>
+      <c r="H38">
+        <v>-27</v>
+      </c>
+      <c r="I38">
+        <v>89</v>
+      </c>
+      <c r="K38" t="s">
+        <v>17</v>
+      </c>
+      <c r="M38">
+        <v>60</v>
+      </c>
+      <c r="N38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40">
+        <v>0.2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>126</v>
+      </c>
+      <c r="G40">
+        <v>0.11</v>
+      </c>
+      <c r="H40">
+        <v>-140</v>
+      </c>
+      <c r="I40">
+        <v>94</v>
+      </c>
+      <c r="J40">
+        <v>126</v>
+      </c>
+      <c r="K40" t="s">
+        <v>17</v>
+      </c>
+      <c r="M40">
+        <v>60</v>
+      </c>
+      <c r="N40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41">
+        <v>0.25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>116</v>
+      </c>
+      <c r="G41">
+        <v>0.11</v>
+      </c>
+      <c r="H41">
+        <v>30</v>
+      </c>
+      <c r="I41">
+        <v>91</v>
+      </c>
+      <c r="J41">
+        <v>539</v>
+      </c>
+      <c r="K41" t="s">
+        <v>7</v>
+      </c>
+      <c r="M41">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>98</v>
+      </c>
+      <c r="G47" t="s">
+        <v>98</v>
+      </c>
+      <c r="H47">
+        <v>58</v>
+      </c>
+      <c r="I47">
+        <v>126</v>
+      </c>
+      <c r="K47" t="s">
+        <v>7</v>
+      </c>
+      <c r="M47">
+        <v>60</v>
+      </c>
+      <c r="N47" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G48" t="s">
+        <v>98</v>
+      </c>
+      <c r="H48">
+        <v>-55</v>
+      </c>
+      <c r="I48">
+        <v>39</v>
+      </c>
+      <c r="K48" t="s">
+        <v>17</v>
+      </c>
+      <c r="M48">
+        <v>60</v>
+      </c>
+      <c r="N48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>98</v>
+      </c>
+      <c r="G50" t="s">
+        <v>98</v>
+      </c>
+      <c r="H50">
+        <v>58</v>
+      </c>
+      <c r="I50">
+        <v>126</v>
+      </c>
+      <c r="J50">
+        <v>519</v>
+      </c>
+      <c r="K50" t="s">
+        <v>7</v>
+      </c>
+      <c r="M50">
+        <v>60</v>
+      </c>
+      <c r="N50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>98</v>
+      </c>
+      <c r="G51" t="s">
+        <v>98</v>
+      </c>
+      <c r="H51">
+        <v>73</v>
+      </c>
+      <c r="I51">
+        <v>257</v>
+      </c>
+      <c r="J51">
+        <v>685</v>
+      </c>
+      <c r="K51" t="s">
+        <v>134</v>
+      </c>
+      <c r="M51">
+        <v>60</v>
+      </c>
+      <c r="N51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>37</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B53" t="s">
         <v>40</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C53" t="s">
         <v>40</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D53" t="s">
         <v>38</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F53" t="s">
         <v>39</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G53" t="s">
         <v>41</v>
       </c>
-      <c r="H41">
+      <c r="H53">
         <f>249/1.6/1.5</f>
         <v>103.75</v>
       </c>
-      <c r="I41">
+      <c r="I53">
         <f>1170/1.6/1.5*3600/1000</f>
         <v>1755</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K53" t="s">
         <v>47</v>
       </c>
-      <c r="L41">
+      <c r="L53">
         <f>333000/1.6/1.5</f>
         <v>138750</v>
       </c>
-      <c r="M41">
+      <c r="M53">
         <v>30</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N53" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>37</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B54" t="s">
         <v>44</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C54" t="s">
         <v>44</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D54" t="s">
         <v>49</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F54" t="s">
         <v>48</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G54" t="s">
         <v>45</v>
       </c>
-      <c r="H42">
+      <c r="H54">
         <f>392/1.5/1.6</f>
         <v>163.33333333333331</v>
       </c>
-      <c r="I42">
+      <c r="I54">
         <f>1740/1.6/1.5*3600/1000</f>
         <v>2610</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K54" t="s">
         <v>46</v>
       </c>
-      <c r="L42">
+      <c r="L54">
         <f>440000/1.5/1.6</f>
         <v>183333.33333333331</v>
       </c>
-      <c r="M42">
+      <c r="M54">
         <v>30</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N54" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>37</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B56" t="s">
         <v>76</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C56" t="s">
         <v>79</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D56" t="s">
         <v>87</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F56" t="s">
         <v>48</v>
       </c>
-      <c r="G44">
+      <c r="G56">
         <v>1.3</v>
       </c>
-      <c r="H44">
+      <c r="H56">
         <v>206</v>
       </c>
-      <c r="I44">
+      <c r="I56">
         <v>1150</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K56" t="s">
         <v>81</v>
       </c>
-      <c r="L44">
+      <c r="L56">
         <v>307000</v>
       </c>
-      <c r="M44">
+      <c r="M56">
         <v>30</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="N56" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>37</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B57" t="s">
         <v>77</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C57" t="s">
         <v>80</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D57" t="s">
         <v>88</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F57" t="s">
         <v>83</v>
       </c>
-      <c r="G45">
+      <c r="G57">
         <v>0.9</v>
       </c>
-      <c r="H45">
+      <c r="H57">
         <v>272</v>
       </c>
-      <c r="I45">
+      <c r="I57">
         <v>1520</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K57" t="s">
         <v>81</v>
       </c>
-      <c r="L45">
+      <c r="L57">
         <v>399000</v>
       </c>
-      <c r="M45">
+      <c r="M57">
         <v>30</v>
       </c>
-      <c r="N45" s="2" t="s">
+      <c r="N57" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>37</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B58" t="s">
         <v>78</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C58" t="s">
         <v>80</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D58" t="s">
         <v>89</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F58" t="s">
         <v>84</v>
       </c>
-      <c r="G46">
+      <c r="G58">
         <v>0.74</v>
       </c>
-      <c r="H46">
+      <c r="H58">
         <v>287</v>
       </c>
-      <c r="I46">
+      <c r="I58">
         <v>1630</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K58" t="s">
         <v>81</v>
       </c>
-      <c r="L46">
+      <c r="L58">
         <v>422000</v>
       </c>
-      <c r="M46">
+      <c r="M58">
         <v>30</v>
       </c>
-      <c r="N46" s="2" t="s">
+      <c r="N58" s="2" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
detailed envelope embodied emission storage
</commit_message>
<xml_diff>
--- a/data/embodied_emissions_envelope.xlsx
+++ b/data/embodied_emissions_envelope.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LW_Simulation\PycharmProjects\sia_380-1-full_version\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandra/Desktop/Master Thesis/02 Edits/02 Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03574D8C-3E0C-BA40-8FFC-2B2B5A0968AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31245" yWindow="4905" windowWidth="27675" windowHeight="17040"/>
+    <workbookView xWindow="31520" yWindow="-3480" windowWidth="27680" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="177">
   <si>
     <t>Abk</t>
   </si>
@@ -504,19 +505,86 @@
   </si>
   <si>
     <t>UBP[/m2]</t>
+  </si>
+  <si>
+    <t>W_BC2</t>
+  </si>
+  <si>
+    <t>Wi_BC2</t>
+  </si>
+  <si>
+    <t>F_BC2</t>
+  </si>
+  <si>
+    <t>R_BC2</t>
+  </si>
+  <si>
+    <t>Window_BC2</t>
+  </si>
+  <si>
+    <t>Floor_BC2</t>
+  </si>
+  <si>
+    <t>Roof_BC2</t>
+  </si>
+  <si>
+    <t>Gypsum_Concrete_Bitumen_PUR_Bitumen_Rubber_Stones</t>
+  </si>
+  <si>
+    <t>Gypsum_Concrete_Bitumen_PUR_PE_Timber_PVA_PE_Steel</t>
+  </si>
+  <si>
+    <t>R_SIA380_1</t>
+  </si>
+  <si>
+    <t>R_SIA380_2</t>
+  </si>
+  <si>
+    <t>mix between R_SIA380_1 and R_SIA380_2</t>
+  </si>
+  <si>
+    <t>PUR PIR</t>
+  </si>
+  <si>
+    <t>MFH 4, John (2012) https://www.research-collection.ethz.ch/handle/20.500.11850/64978</t>
+  </si>
+  <si>
+    <t>Wall_BC2</t>
+  </si>
+  <si>
+    <t>Ceiling_BC2</t>
+  </si>
+  <si>
+    <t>ceiling</t>
+  </si>
+  <si>
+    <t>C_BC2</t>
+  </si>
+  <si>
+    <t>Cement_Concrete_PE_Concrete</t>
+  </si>
+  <si>
+    <t>GraniteFloor_Cement_PE_EPS_Concrete_Gypsum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -532,6 +600,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -556,16 +631,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -587,7 +664,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -624,7 +701,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -650,7 +726,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1046,7 +1122,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1072,7 +1147,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1110,7 +1185,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484269216"/>
@@ -1164,7 +1239,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1190,7 +1264,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1228,7 +1302,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484262328"/>
@@ -1268,7 +1342,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1294,7 +1367,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1332,7 +1405,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="481821672"/>
@@ -1364,7 +1437,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1390,7 +1462,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1420,7 +1492,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1434,7 +1506,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1471,7 +1543,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1497,7 +1568,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1893,7 +1964,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1919,7 +1989,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1957,7 +2027,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484269216"/>
@@ -2016,7 +2086,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2042,7 +2111,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2080,7 +2149,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484262328"/>
@@ -2120,7 +2189,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2146,7 +2214,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2184,7 +2252,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="503947576"/>
@@ -2216,7 +2284,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2242,7 +2309,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2272,7 +2339,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3401,14 +3468,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>445770</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>49530</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3436,15 +3503,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>11430</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1065530</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3736,29 +3803,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="79.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="79.83203125" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="32.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
     <col min="8" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" customWidth="1"/>
     <col min="12" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -3802,7 +3869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -3847,7 +3914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3892,7 +3959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -3937,7 +4004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -3982,7 +4049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -4027,7 +4094,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -4072,7 +4139,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -4117,7 +4184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -4162,7 +4229,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -4207,7 +4274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -4252,7 +4319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -4297,7 +4364,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -4342,7 +4409,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -4387,7 +4454,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -4432,7 +4499,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -4477,7 +4544,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -4522,12 +4589,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -4559,7 +4626,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -4591,7 +4658,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -4629,7 +4696,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -4667,7 +4734,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -4705,7 +4772,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -4743,7 +4810,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -4781,7 +4848,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -4819,7 +4886,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -4857,7 +4924,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -4880,13 +4947,13 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="H30" s="6">
-        <v>272.39999999999998</v>
+        <v>189.9</v>
       </c>
       <c r="K30" t="s">
         <v>7</v>
       </c>
       <c r="L30">
-        <v>169183</v>
+        <v>190633</v>
       </c>
       <c r="M30">
         <v>60</v>
@@ -4895,7 +4962,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4921,14 +4988,14 @@
       </c>
       <c r="H31" s="6">
         <f>1068*H29/(1068+310)+310*H30/(1068+310)</f>
-        <v>152.65689404934687</v>
+        <v>134.09738751814223</v>
       </c>
       <c r="K31" t="s">
         <v>143</v>
       </c>
       <c r="L31" s="6">
         <f>1068*L29/(1068+310)+310*L30/(1068+310)</f>
-        <v>106334.53265602322</v>
+        <v>111160.00435413643</v>
       </c>
       <c r="M31">
         <v>60</v>
@@ -4937,76 +5004,76 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G32" s="3"/>
-      <c r="H32" s="6"/>
-      <c r="L32" s="6"/>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="H32" s="6">
+        <v>105.2</v>
+      </c>
+      <c r="K32" t="s">
+        <v>119</v>
+      </c>
+      <c r="L32" s="6">
+        <v>84417</v>
+      </c>
+      <c r="M32">
+        <v>60</v>
+      </c>
+      <c r="N32" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34">
-        <v>0.16</v>
-      </c>
-      <c r="F34" t="s">
-        <v>63</v>
-      </c>
-      <c r="G34">
-        <v>0.19</v>
-      </c>
-      <c r="H34">
-        <v>71</v>
-      </c>
-      <c r="I34">
-        <v>196</v>
-      </c>
-      <c r="K34" t="s">
-        <v>7</v>
-      </c>
-      <c r="M34">
-        <v>60</v>
-      </c>
-      <c r="N34" t="s">
-        <v>64</v>
-      </c>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G33" s="3"/>
+      <c r="H33" s="6"/>
+      <c r="L33" s="6"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
         <v>59</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35">
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
       <c r="F35" t="s">
         <v>63</v>
       </c>
       <c r="G35">
-        <v>0.13</v>
+        <v>0.19</v>
       </c>
       <c r="H35">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I35">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="K35" t="s">
         <v>7</v>
@@ -5018,33 +5085,33 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
         <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36">
-        <v>0.28000000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="F36" t="s">
         <v>63</v>
       </c>
       <c r="G36">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="H36">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I36">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="K36" t="s">
         <v>7</v>
@@ -5056,36 +5123,36 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E37">
-        <v>0.15</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F37" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="G37">
-        <v>0.25</v>
+        <v>0.11</v>
       </c>
       <c r="H37">
-        <v>-22</v>
+        <v>76</v>
       </c>
       <c r="I37">
-        <v>68</v>
+        <v>239</v>
       </c>
       <c r="K37" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="M37">
         <v>60</v>
@@ -5094,33 +5161,33 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
         <v>102</v>
       </c>
       <c r="D38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E38">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="F38" t="s">
         <v>108</v>
       </c>
       <c r="G38">
-        <v>0.14000000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="H38">
-        <v>-26</v>
+        <v>-22</v>
       </c>
       <c r="I38">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="K38" t="s">
         <v>16</v>
@@ -5132,33 +5199,33 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
         <v>102</v>
       </c>
       <c r="D39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E39">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="F39" t="s">
         <v>108</v>
       </c>
       <c r="G39">
-        <v>0.12</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H39">
-        <v>-27</v>
+        <v>-26</v>
       </c>
       <c r="I39">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K39" t="s">
         <v>16</v>
@@ -5170,74 +5237,74 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>68</v>
       </c>
-      <c r="B41" t="s">
-        <v>135</v>
-      </c>
-      <c r="C41" t="s">
-        <v>116</v>
-      </c>
-      <c r="D41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E41">
-        <v>0.16</v>
-      </c>
-      <c r="F41" t="s">
-        <v>141</v>
-      </c>
-      <c r="G41">
-        <v>0.16</v>
-      </c>
-      <c r="H41">
-        <v>158.6</v>
-      </c>
-      <c r="K41" t="s">
-        <v>7</v>
-      </c>
-      <c r="L41">
-        <v>181139</v>
-      </c>
-      <c r="M41">
+      <c r="B40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40">
+        <v>0.32</v>
+      </c>
+      <c r="F40" t="s">
+        <v>108</v>
+      </c>
+      <c r="G40">
+        <v>0.12</v>
+      </c>
+      <c r="H40">
+        <v>-27</v>
+      </c>
+      <c r="I40">
+        <v>89</v>
+      </c>
+      <c r="K40" t="s">
+        <v>16</v>
+      </c>
+      <c r="M40">
         <v>60</v>
       </c>
-      <c r="N41" t="s">
-        <v>120</v>
+      <c r="N40" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C42" t="s">
         <v>116</v>
       </c>
       <c r="D42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E42">
-        <v>0.32</v>
+        <v>0.16</v>
       </c>
       <c r="F42" t="s">
         <v>141</v>
       </c>
       <c r="G42">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="H42">
-        <v>186.8</v>
+        <v>158.6</v>
       </c>
       <c r="K42" t="s">
         <v>7</v>
       </c>
       <c r="L42">
-        <v>210730</v>
+        <v>181139</v>
       </c>
       <c r="M42">
         <v>60</v>
@@ -5246,562 +5313,827 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
-      </c>
-      <c r="E43" s="3">
-        <f>250*E41/(250+460)+460*E42/(250+460)</f>
-        <v>0.26366197183098594</v>
+        <v>140</v>
+      </c>
+      <c r="E43">
+        <v>0.32</v>
       </c>
       <c r="F43" t="s">
         <v>141</v>
       </c>
-      <c r="G43" s="3">
-        <f>250*G41/(250+460)+460*G42/(250+460)</f>
-        <v>0.12112676056338029</v>
-      </c>
-      <c r="H43" s="3">
-        <f>250*H41/(250+460)+460*H42/(250+460)</f>
-        <v>176.87042253521128</v>
+      <c r="G43">
+        <v>0.1</v>
+      </c>
+      <c r="H43">
+        <v>186.8</v>
       </c>
       <c r="K43" t="s">
         <v>7</v>
       </c>
-      <c r="L43" s="6">
-        <f>250*L41/(250+460)+460*L42/(250+460)</f>
-        <v>200310.63380281688</v>
+      <c r="L43">
+        <v>210730</v>
       </c>
       <c r="M43">
         <v>60</v>
       </c>
       <c r="N43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44" s="3">
+        <f>250*E42/(250+460)+460*E43/(250+460)</f>
+        <v>0.26366197183098594</v>
+      </c>
+      <c r="F44" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="3">
+        <f>250*G42/(250+460)+460*G43/(250+460)</f>
+        <v>0.12112676056338029</v>
+      </c>
+      <c r="H44" s="3">
+        <f>250*H42/(250+460)+460*H43/(250+460)</f>
+        <v>176.87042253521128</v>
+      </c>
+      <c r="K44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L44" s="6">
+        <f>250*L42/(250+460)+460*L43/(250+460)</f>
+        <v>200310.63380281688</v>
+      </c>
+      <c r="M44">
+        <v>60</v>
+      </c>
+      <c r="N44" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45">
+        <v>0.16</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="H45" s="3">
+        <v>160.6</v>
+      </c>
+      <c r="K45" t="s">
+        <v>7</v>
+      </c>
+      <c r="L45" s="6">
+        <v>196764</v>
+      </c>
+      <c r="M45">
+        <v>60</v>
+      </c>
+      <c r="N45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" t="s">
-        <v>109</v>
+        <v>68</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D46" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46" t="s">
-        <v>98</v>
-      </c>
-      <c r="G46" t="s">
-        <v>98</v>
-      </c>
-      <c r="H46">
-        <v>58</v>
-      </c>
-      <c r="I46">
-        <v>126</v>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="H46" s="3">
+        <v>178.5</v>
       </c>
       <c r="K46" t="s">
         <v>7</v>
       </c>
+      <c r="L46" s="6">
+        <v>363719</v>
+      </c>
       <c r="M46">
         <v>60</v>
       </c>
       <c r="N46" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>110</v>
+        <v>163</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
+        <v>160</v>
+      </c>
+      <c r="E47" s="4">
+        <f>126.7*E45/(126.7+140)+140*E46/(126.7+140)</f>
+        <v>0.14950131233595804</v>
       </c>
       <c r="F47" t="s">
-        <v>98</v>
-      </c>
-      <c r="G47" t="s">
-        <v>98</v>
-      </c>
-      <c r="H47">
-        <v>-55</v>
-      </c>
-      <c r="I47">
-        <v>39</v>
+        <v>169</v>
+      </c>
+      <c r="G47" s="8">
+        <f>126.7*G45/(126.7+140)+140*G46/(126.7+140)</f>
+        <v>0.16149606299212599</v>
+      </c>
+      <c r="H47" s="6">
+        <f>126.7*H45/(126.7+140)+140*H46/(126.7+140)</f>
+        <v>169.99632545931757</v>
       </c>
       <c r="K47" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="L47" s="6">
+        <f>126.7*L45/(126.7+140)+140*L46/(126.7+140)</f>
+        <v>284404.41994750657</v>
       </c>
       <c r="M47">
         <v>60</v>
       </c>
       <c r="N47" t="s">
-        <v>112</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>96</v>
-      </c>
-      <c r="B49" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" t="s">
-        <v>116</v>
-      </c>
-      <c r="D49" t="s">
-        <v>128</v>
-      </c>
-      <c r="E49">
-        <v>0.3</v>
-      </c>
-      <c r="F49" t="s">
-        <v>142</v>
-      </c>
-      <c r="G49">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="H49">
-        <v>128.5</v>
-      </c>
-      <c r="K49" t="s">
-        <v>7</v>
-      </c>
-      <c r="L49">
-        <v>162903</v>
-      </c>
-      <c r="M49">
-        <v>60</v>
-      </c>
-      <c r="N49" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>96</v>
       </c>
       <c r="B50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>98</v>
+      </c>
+      <c r="G50" t="s">
+        <v>98</v>
+      </c>
+      <c r="H50">
+        <v>58</v>
+      </c>
+      <c r="I50">
         <v>126</v>
-      </c>
-      <c r="C50" t="s">
-        <v>116</v>
-      </c>
-      <c r="D50" t="s">
-        <v>129</v>
-      </c>
-      <c r="E50">
-        <v>0.3</v>
-      </c>
-      <c r="F50" t="s">
-        <v>142</v>
-      </c>
-      <c r="G50">
-        <v>0.16</v>
-      </c>
-      <c r="H50">
-        <v>167.8</v>
       </c>
       <c r="K50" t="s">
         <v>7</v>
       </c>
-      <c r="L50">
-        <v>205504</v>
-      </c>
       <c r="M50">
         <v>60</v>
       </c>
       <c r="N50" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>96</v>
       </c>
       <c r="B51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>98</v>
+      </c>
+      <c r="G51" t="s">
+        <v>98</v>
+      </c>
+      <c r="H51">
+        <v>-55</v>
+      </c>
+      <c r="I51">
+        <v>39</v>
+      </c>
+      <c r="K51" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51">
+        <v>60</v>
+      </c>
+      <c r="N51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53">
+        <v>0.3</v>
+      </c>
+      <c r="F53" t="s">
+        <v>142</v>
+      </c>
+      <c r="G53">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H53">
+        <v>117.1</v>
+      </c>
+      <c r="K53" t="s">
+        <v>7</v>
+      </c>
+      <c r="L53">
+        <v>152763</v>
+      </c>
+      <c r="M53">
+        <v>60</v>
+      </c>
+      <c r="N53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54">
+        <v>0.3</v>
+      </c>
+      <c r="F54" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54">
+        <v>0.16</v>
+      </c>
+      <c r="H54">
+        <v>162.80000000000001</v>
+      </c>
+      <c r="K54" t="s">
+        <v>7</v>
+      </c>
+      <c r="L54">
+        <v>206295</v>
+      </c>
+      <c r="M54">
+        <v>60</v>
+      </c>
+      <c r="N54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" t="s">
         <v>131</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C55" t="s">
         <v>138</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D55" t="s">
         <v>130</v>
       </c>
-      <c r="E51" s="5">
-        <f>387*E49/(387+242)+242*E50/(387+242)</f>
+      <c r="E55" s="5">
+        <f>387*E53/(387+242)+242*E54/(387+242)</f>
         <v>0.3</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F55" t="s">
         <v>142</v>
       </c>
-      <c r="G51" s="4">
-        <f>387*G49/(387+242)+242*G50/(387+242)</f>
+      <c r="G55" s="4">
+        <f>387*G53/(387+242)+242*G54/(387+242)</f>
         <v>0.23383147853736092</v>
       </c>
-      <c r="H51" s="3">
-        <f>387*H49/(387+242)+242*H50/(387+242)</f>
-        <v>143.62019077901431</v>
-      </c>
-      <c r="K51" t="s">
+      <c r="H55" s="3">
+        <f>387*H53/(387+242)+242*H54/(387+242)</f>
+        <v>134.68251192368839</v>
+      </c>
+      <c r="K55" t="s">
         <v>7</v>
       </c>
-      <c r="L51" s="6">
-        <f>387*L49/(387+242)+242*L50/(387+242)</f>
-        <v>179293.20985691575</v>
-      </c>
-      <c r="M51" s="6">
-        <f>387*M49/(387+242)+242*M50/(387+242)</f>
+      <c r="L55" s="6">
+        <f>387*L53/(387+242)+242*L54/(387+242)</f>
+        <v>173358.7774244833</v>
+      </c>
+      <c r="M55" s="6">
+        <f>387*M53/(387+242)+242*M54/(387+242)</f>
         <v>60</v>
       </c>
-      <c r="N51" t="s">
+      <c r="N55" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E52" s="5"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="3"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" t="s">
+        <v>162</v>
+      </c>
+      <c r="C56" t="s">
+        <v>175</v>
+      </c>
+      <c r="D56" t="s">
+        <v>159</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F56" t="s">
+        <v>98</v>
+      </c>
+      <c r="G56" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="H56" s="3">
+        <v>105.6</v>
+      </c>
+      <c r="K56" t="s">
+        <v>7</v>
+      </c>
+      <c r="L56" s="6">
+        <v>143901</v>
+      </c>
+      <c r="M56" s="6">
+        <v>60</v>
+      </c>
+      <c r="N56" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" t="s">
+        <v>172</v>
+      </c>
+      <c r="C57" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" t="s">
+        <v>174</v>
+      </c>
+      <c r="E57" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="F57" t="s">
+        <v>63</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H57" s="3">
+        <v>114.4</v>
+      </c>
+      <c r="K57" t="s">
+        <v>7</v>
+      </c>
+      <c r="L57" s="6">
+        <v>154647</v>
+      </c>
+      <c r="M57" s="6">
+        <v>60</v>
+      </c>
+      <c r="N57" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>36</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B59" t="s">
         <v>39</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C59" t="s">
         <v>39</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D59" t="s">
         <v>37</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F59" t="s">
         <v>38</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G59" t="s">
         <v>40</v>
       </c>
-      <c r="H54">
+      <c r="H59">
         <f>249/1.6/1.5</f>
         <v>103.75</v>
       </c>
-      <c r="I54">
+      <c r="I59">
         <f>1170/1.6/1.5*3600/1000</f>
         <v>1755</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K59" t="s">
         <v>46</v>
       </c>
-      <c r="L54">
+      <c r="L59">
         <f>333000/1.6/1.5</f>
         <v>138750</v>
       </c>
-      <c r="M54">
+      <c r="M59">
         <v>30</v>
       </c>
-      <c r="N54" s="2" t="s">
+      <c r="N59" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>36</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B60" t="s">
         <v>43</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C60" t="s">
         <v>43</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D60" t="s">
         <v>48</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F60" t="s">
         <v>47</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G60" t="s">
         <v>44</v>
       </c>
-      <c r="H55" s="4">
+      <c r="H60" s="4">
         <f>392/1.5/1.6</f>
         <v>163.33333333333331</v>
       </c>
-      <c r="I55">
+      <c r="I60">
         <f>1740/1.6/1.5*3600/1000</f>
         <v>2610</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K60" t="s">
         <v>45</v>
       </c>
-      <c r="L55" s="6">
+      <c r="L60" s="6">
         <f>440000/1.5/1.6</f>
         <v>183333.33333333331</v>
       </c>
-      <c r="M55">
+      <c r="M60">
         <v>30</v>
       </c>
-      <c r="N55" t="s">
+      <c r="N60" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57" t="s">
-        <v>75</v>
-      </c>
-      <c r="C57" t="s">
-        <v>78</v>
-      </c>
-      <c r="D57" t="s">
-        <v>86</v>
-      </c>
-      <c r="F57" t="s">
-        <v>47</v>
-      </c>
-      <c r="G57">
-        <v>1.3</v>
-      </c>
-      <c r="H57">
-        <v>206</v>
-      </c>
-      <c r="I57">
-        <v>1150</v>
-      </c>
-      <c r="K57" t="s">
-        <v>80</v>
-      </c>
-      <c r="L57">
-        <v>307000</v>
-      </c>
-      <c r="M57">
-        <v>30</v>
-      </c>
-      <c r="N57" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>36</v>
-      </c>
-      <c r="B58" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" t="s">
-        <v>79</v>
-      </c>
-      <c r="D58" t="s">
-        <v>87</v>
-      </c>
-      <c r="F58" t="s">
-        <v>82</v>
-      </c>
-      <c r="G58">
-        <v>0.9</v>
-      </c>
-      <c r="H58">
-        <v>272</v>
-      </c>
-      <c r="I58">
-        <v>1520</v>
-      </c>
-      <c r="K58" t="s">
-        <v>80</v>
-      </c>
-      <c r="L58">
-        <v>399000</v>
-      </c>
-      <c r="M58">
-        <v>30</v>
-      </c>
-      <c r="N58" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>36</v>
-      </c>
-      <c r="B59" t="s">
-        <v>77</v>
-      </c>
-      <c r="C59" t="s">
-        <v>79</v>
-      </c>
-      <c r="D59" t="s">
-        <v>88</v>
-      </c>
-      <c r="F59" t="s">
-        <v>83</v>
-      </c>
-      <c r="G59">
-        <v>0.74</v>
-      </c>
-      <c r="H59">
-        <v>287</v>
-      </c>
-      <c r="I59">
-        <v>1630</v>
-      </c>
-      <c r="K59" t="s">
-        <v>80</v>
-      </c>
-      <c r="L59">
-        <v>422000</v>
-      </c>
-      <c r="M59">
-        <v>30</v>
-      </c>
-      <c r="N59" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>36</v>
-      </c>
-      <c r="B61" t="s">
-        <v>145</v>
-      </c>
-      <c r="C61" t="s">
-        <v>146</v>
-      </c>
-      <c r="D61" t="s">
-        <v>147</v>
-      </c>
-      <c r="F61" t="s">
-        <v>38</v>
-      </c>
-      <c r="G61">
-        <v>0.9</v>
-      </c>
-      <c r="H61" s="6">
-        <f>491/1.75/1.3</f>
-        <v>215.8241758241758</v>
-      </c>
-      <c r="K61" t="s">
-        <v>148</v>
-      </c>
-      <c r="L61" s="6">
-        <f>898000/1.75/1.3</f>
-        <v>394725.27472527471</v>
-      </c>
-      <c r="M61">
-        <v>30</v>
-      </c>
-      <c r="N61" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>36</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="C62" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="D62" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="F62" t="s">
         <v>47</v>
       </c>
       <c r="G62">
-        <v>1.23</v>
-      </c>
-      <c r="H62" s="6">
-        <f>555/1.75/1.3</f>
-        <v>243.95604395604397</v>
+        <v>1.3</v>
+      </c>
+      <c r="H62">
+        <v>206</v>
+      </c>
+      <c r="I62">
+        <v>1150</v>
       </c>
       <c r="K62" t="s">
-        <v>148</v>
-      </c>
-      <c r="L62" s="6">
-        <f>1100000/1.75/1.3</f>
-        <v>483516.48351648345</v>
+        <v>80</v>
+      </c>
+      <c r="L62">
+        <v>307000</v>
       </c>
       <c r="M62">
         <v>30</v>
       </c>
-      <c r="N62" t="s">
-        <v>149</v>
+      <c r="N62" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>36</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="D63" t="s">
-        <v>155</v>
-      </c>
-      <c r="G63" s="4">
-        <f>393*G61/(393+58)+58*G62/(393+58)</f>
-        <v>0.94243902439024385</v>
-      </c>
-      <c r="H63" s="6">
-        <f>393*H61/(393+58)+58*H62/(393+58)</f>
-        <v>219.44202139324088</v>
+        <v>87</v>
+      </c>
+      <c r="F63" t="s">
+        <v>82</v>
+      </c>
+      <c r="G63">
+        <v>0.9</v>
+      </c>
+      <c r="H63">
+        <v>272</v>
+      </c>
+      <c r="I63">
+        <v>1520</v>
       </c>
       <c r="K63" t="s">
-        <v>148</v>
-      </c>
-      <c r="L63" s="6">
-        <f>393*L61/(393+58)+58*L62/(393+58)</f>
-        <v>406144.09980263637</v>
+        <v>80</v>
+      </c>
+      <c r="L63">
+        <v>399000</v>
       </c>
       <c r="M63">
         <v>30</v>
       </c>
-      <c r="N63" t="s">
+      <c r="N63" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" t="s">
+        <v>83</v>
+      </c>
+      <c r="G64">
+        <v>0.74</v>
+      </c>
+      <c r="H64">
+        <v>287</v>
+      </c>
+      <c r="I64">
+        <v>1630</v>
+      </c>
+      <c r="K64" t="s">
+        <v>80</v>
+      </c>
+      <c r="L64">
+        <v>422000</v>
+      </c>
+      <c r="M64">
+        <v>30</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" t="s">
+        <v>145</v>
+      </c>
+      <c r="C66" t="s">
+        <v>146</v>
+      </c>
+      <c r="D66" t="s">
+        <v>147</v>
+      </c>
+      <c r="F66" t="s">
+        <v>38</v>
+      </c>
+      <c r="G66">
+        <v>0.9</v>
+      </c>
+      <c r="H66" s="6">
+        <f>276/1.75/1.3</f>
+        <v>121.31868131868131</v>
+      </c>
+      <c r="K66" t="s">
+        <v>148</v>
+      </c>
+      <c r="L66" s="6">
+        <f>352000/1.75/1.3</f>
+        <v>154725.27472527471</v>
+      </c>
+      <c r="M66">
+        <v>30</v>
+      </c>
+      <c r="N66" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" t="s">
+        <v>152</v>
+      </c>
+      <c r="F67" t="s">
+        <v>47</v>
+      </c>
+      <c r="G67">
+        <v>1.23</v>
+      </c>
+      <c r="H67" s="6">
+        <f>220/1.75/1.3</f>
+        <v>96.703296703296701</v>
+      </c>
+      <c r="K67" t="s">
+        <v>148</v>
+      </c>
+      <c r="L67" s="6">
+        <f>291000/1.75/1.3</f>
+        <v>127912.08791208791</v>
+      </c>
+      <c r="M67">
+        <v>30</v>
+      </c>
+      <c r="N67" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" t="s">
+        <v>154</v>
+      </c>
+      <c r="D68" t="s">
+        <v>155</v>
+      </c>
+      <c r="G68" s="4">
+        <f>393*G66/(393+58)+58*G67/(393+58)</f>
+        <v>0.94243902439024385</v>
+      </c>
+      <c r="H68" s="6">
+        <f>393*H66/(393+58)+58*H67/(393+58)</f>
+        <v>118.15306644574936</v>
+      </c>
+      <c r="K68" t="s">
+        <v>148</v>
+      </c>
+      <c r="L68" s="6">
+        <f>393*L66/(393+58)+58*L67/(393+58)</f>
+        <v>151277.01566725958</v>
+      </c>
+      <c r="M68">
+        <v>30</v>
+      </c>
+      <c r="N68" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>36</v>
+      </c>
+      <c r="B69" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" t="s">
+        <v>158</v>
+      </c>
+      <c r="F69" t="s">
+        <v>47</v>
+      </c>
+      <c r="G69">
+        <v>1.3</v>
+      </c>
+      <c r="H69" s="6">
+        <f>220/1.75/1.3</f>
+        <v>96.703296703296701</v>
+      </c>
+      <c r="K69" t="s">
+        <v>148</v>
+      </c>
+      <c r="L69" s="6">
+        <f>291000/1.75/1.3</f>
+        <v>127912.08791208791</v>
+      </c>
+      <c r="M69">
+        <v>30</v>
+      </c>
+      <c r="N69" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N54" r:id="rId1"/>
+    <hyperlink ref="N59" r:id="rId1" xr:uid="{61032813-A891-F145-949A-3FC78FBCD676}"/>
+    <hyperlink ref="N66" r:id="rId2" xr:uid="{9A37C0FD-BB04-014B-BFC0-4A028B31EFB5}"/>
+    <hyperlink ref="N67" r:id="rId3" xr:uid="{E7FC74C7-197C-9E4B-BF0B-5F1705E181B5}"/>
+    <hyperlink ref="N69" r:id="rId4" xr:uid="{470944A1-1EDF-7C46-BF0C-F1995000D973}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KBOB coefficients nutzwärme --> endenergie
</commit_message>
<xml_diff>
--- a/data/embodied_emissions_envelope.xlsx
+++ b/data/embodied_emissions_envelope.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandra/Desktop/Master Thesis/02 Edits/02 Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandra/Desktop/Master_Thesis/02_Edits/02_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03574D8C-3E0C-BA40-8FFC-2B2B5A0968AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7D4183-178E-AF41-BFE4-786D504BE964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31520" yWindow="-3480" windowWidth="27680" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="236">
   <si>
     <t>Abk</t>
   </si>
@@ -565,6 +565,183 @@
   </si>
   <si>
     <t>GraniteFloor_Cement_PE_EPS_Concrete_Gypsum</t>
+  </si>
+  <si>
+    <t>Zellulosedämmplatte</t>
+  </si>
+  <si>
+    <t>Schaumglas</t>
+  </si>
+  <si>
+    <t>Renovation</t>
+  </si>
+  <si>
+    <t>Ren_18_glasswool</t>
+  </si>
+  <si>
+    <t>Ren_13_stonewool</t>
+  </si>
+  <si>
+    <t>Ren_18_stonewool</t>
+  </si>
+  <si>
+    <t>Ren_13_EPS</t>
+  </si>
+  <si>
+    <t>Ren_18_EPS</t>
+  </si>
+  <si>
+    <t>Ren_13_XPS</t>
+  </si>
+  <si>
+    <t>Ren_18_XPS</t>
+  </si>
+  <si>
+    <t>Ren_8_PU</t>
+  </si>
+  <si>
+    <t>Ren_13_PU</t>
+  </si>
+  <si>
+    <t>Ren_13_foamglass</t>
+  </si>
+  <si>
+    <t>Ren_18_foamglass</t>
+  </si>
+  <si>
+    <t>Ren_13_cellulose</t>
+  </si>
+  <si>
+    <t>Ren_18_cellulose</t>
+  </si>
+  <si>
+    <t>Wi_3_Ren</t>
+  </si>
+  <si>
+    <t>3 fach Verglasung mit Entsorgung altes Fenster</t>
+  </si>
+  <si>
+    <t>3fach Verglasung HolzAlu plus Entsorgung altes Fenster (2fach, Holz, Entsorgung), Fensterrechner treeze</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>Ren_13_glasswool</t>
+  </si>
+  <si>
+    <t>Insulation 11-15cm Glass Wool</t>
+  </si>
+  <si>
+    <t>Insulation 16-20cm Glass Wool</t>
+  </si>
+  <si>
+    <t>Insulation 11-15cm Stone Wool</t>
+  </si>
+  <si>
+    <t>Insulation 16-20cm Stone Wool</t>
+  </si>
+  <si>
+    <t>Insulation 11-15cm EPS</t>
+  </si>
+  <si>
+    <t>Insulation 16-20cm EPS</t>
+  </si>
+  <si>
+    <t>Insulation 11-15cm XPS</t>
+  </si>
+  <si>
+    <t>Insulation 16-20cm XPS</t>
+  </si>
+  <si>
+    <t>Insulation 6-10cm PU</t>
+  </si>
+  <si>
+    <t>Insulation 11-15cm PU</t>
+  </si>
+  <si>
+    <t>Insulation 11-15cm Foam Glass</t>
+  </si>
+  <si>
+    <t>Insulation 16-20cm Foam Glass</t>
+  </si>
+  <si>
+    <t>Insulation 11-15cm Cellulose</t>
+  </si>
+  <si>
+    <t>Insulation 16-20cm Cellulose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window </t>
+  </si>
+  <si>
+    <t>Ren_8_glasswool</t>
+  </si>
+  <si>
+    <t>Insulation 6-10cm Glass Wool</t>
+  </si>
+  <si>
+    <t>Ren_8_stonewool</t>
+  </si>
+  <si>
+    <t>Insulation 8-10cm Stone Wool</t>
+  </si>
+  <si>
+    <t>Ren_8_EPS</t>
+  </si>
+  <si>
+    <t>Insulation 6-10cm EPS</t>
+  </si>
+  <si>
+    <t>Ren_8_XPS</t>
+  </si>
+  <si>
+    <t>Insulation 6-10cm XPS</t>
+  </si>
+  <si>
+    <t>Roof_SIA380_1</t>
+  </si>
+  <si>
+    <t>Roof_SIA380_2</t>
+  </si>
+  <si>
+    <t>Wall_Aufstockung_D</t>
+  </si>
+  <si>
+    <t>5/6 old wall, 1/6 Aufstockung new wall</t>
+  </si>
+  <si>
+    <t>Renovated_Wall_Aufstockung_D_glasswool</t>
+  </si>
+  <si>
+    <t>Renovated_Wall_Aufstockung_D_XPS</t>
+  </si>
+  <si>
+    <t>5/6 old wall renovated glasswool, 1/6 Aufstockung new wall</t>
+  </si>
+  <si>
+    <t>5/6 old wall renovated XPS, 1/6 Aufstockung new wall</t>
+  </si>
+  <si>
+    <t>glasswool</t>
+  </si>
+  <si>
+    <t>Window_Aufstockung_D</t>
+  </si>
+  <si>
+    <t>5/6 old windows, 1/6 new windows</t>
+  </si>
+  <si>
+    <t>W_Auf_D</t>
+  </si>
+  <si>
+    <t>Ren_W_Auf_D_glasswool</t>
+  </si>
+  <si>
+    <t>Ren_W_Auf_D_XPS</t>
+  </si>
+  <si>
+    <t>Wi_Auf_D</t>
   </si>
 </sst>
 </file>
@@ -575,16 +752,9 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -631,18 +801,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1675,7 +1846,7 @@
             <c:numRef>
               <c:f>Sheet1!$H$2:$H$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.4</c:v>
@@ -2115,7 +2286,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3466,15 +3637,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>445770</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2452370</xdr:colOff>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>49530</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>608330</xdr:colOff>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3502,16 +3673,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1065530</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>303530</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3804,15 +3975,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q75" sqref="Q75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="79.83203125" customWidth="1"/>
     <col min="3" max="3" width="50.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
@@ -3892,7 +4064,7 @@
       <c r="G2">
         <v>0.24</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="6">
         <v>1.4</v>
       </c>
       <c r="I2">
@@ -3937,7 +4109,7 @@
       <c r="G3">
         <v>0.18</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>1.54</v>
       </c>
       <c r="I3">
@@ -3982,7 +4154,7 @@
       <c r="G4">
         <v>0.21</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="6">
         <v>0.5</v>
       </c>
       <c r="I4">
@@ -4027,7 +4199,7 @@
       <c r="G5">
         <v>0.17</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="6">
         <v>0.61</v>
       </c>
       <c r="I5">
@@ -4072,7 +4244,7 @@
       <c r="G6">
         <v>0.21</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
         <v>0.42</v>
       </c>
       <c r="I6">
@@ -4117,7 +4289,7 @@
       <c r="G7">
         <v>0.17</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>0.5</v>
       </c>
       <c r="I7">
@@ -4162,7 +4334,7 @@
       <c r="G8">
         <v>0.21</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="6">
         <v>0.34</v>
       </c>
       <c r="I8">
@@ -4207,7 +4379,7 @@
       <c r="G9">
         <v>0.17</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
         <v>0.39</v>
       </c>
       <c r="I9">
@@ -4252,7 +4424,7 @@
       <c r="G10">
         <v>0.21</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="6">
         <v>2.0299999999999998</v>
       </c>
       <c r="I10">
@@ -4297,7 +4469,7 @@
       <c r="G11">
         <v>0.15</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="6">
         <v>2.27</v>
       </c>
       <c r="I11">
@@ -4342,7 +4514,7 @@
       <c r="G12">
         <v>0.2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="6">
         <v>2.0699999999999998</v>
       </c>
       <c r="I12">
@@ -4387,7 +4559,7 @@
       <c r="G13">
         <v>0.15</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="6">
         <v>2.33</v>
       </c>
       <c r="I13">
@@ -4432,7 +4604,7 @@
       <c r="G14">
         <v>0.2</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="6">
         <v>2</v>
       </c>
       <c r="I14">
@@ -4477,7 +4649,7 @@
       <c r="G15">
         <v>0.15</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="6">
         <v>2.2400000000000002</v>
       </c>
       <c r="I15">
@@ -4522,7 +4694,7 @@
       <c r="G16">
         <v>0.19</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="6">
         <v>2.04</v>
       </c>
       <c r="I16">
@@ -4567,7 +4739,7 @@
       <c r="G17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="6">
         <v>2.29</v>
       </c>
       <c r="I17">
@@ -4589,7 +4761,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="6"/>
       <c r="M18" t="s">
         <v>58</v>
       </c>
@@ -4616,7 +4789,7 @@
       <c r="G19">
         <v>0.2</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="6">
         <v>63</v>
       </c>
       <c r="M19">
@@ -4648,7 +4821,7 @@
       <c r="G20">
         <v>0.11</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="6">
         <v>69</v>
       </c>
       <c r="M20">
@@ -4657,6 +4830,9 @@
       <c r="N20" t="s">
         <v>55</v>
       </c>
+    </row>
+    <row r="21" spans="1:14" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -4680,7 +4856,7 @@
       <c r="G22">
         <v>0.25</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="6">
         <v>63</v>
       </c>
       <c r="I22">
@@ -4718,7 +4894,7 @@
       <c r="G23">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="6">
         <v>67</v>
       </c>
       <c r="I23">
@@ -4756,7 +4932,7 @@
       <c r="G24">
         <v>0.12</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="6">
         <v>69</v>
       </c>
       <c r="I24">
@@ -4794,7 +4970,7 @@
       <c r="G25">
         <v>0.25</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="6">
         <v>-37</v>
       </c>
       <c r="I25">
@@ -4832,7 +5008,7 @@
       <c r="G26">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="6">
         <v>-48</v>
       </c>
       <c r="I26">
@@ -4870,7 +5046,7 @@
       <c r="G27">
         <v>0.12</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="6">
         <v>-55</v>
       </c>
       <c r="I27">
@@ -4885,6 +5061,9 @@
       <c r="N27" t="s">
         <v>64</v>
       </c>
+    </row>
+    <row r="28" spans="1:14" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -5018,22 +5197,22 @@
         <v>157</v>
       </c>
       <c r="E32" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="F32" t="s">
         <v>63</v>
       </c>
       <c r="G32" s="3">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="H32" s="6">
-        <v>105.2</v>
+        <v>109.8</v>
       </c>
       <c r="K32" t="s">
         <v>119</v>
       </c>
       <c r="L32" s="6">
-        <v>84417</v>
+        <v>87525</v>
       </c>
       <c r="M32">
         <v>60</v>
@@ -5043,154 +5222,158 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G33" s="3"/>
-      <c r="H33" s="6"/>
-      <c r="L33" s="6"/>
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D33" t="s">
+        <v>232</v>
+      </c>
+      <c r="E33">
+        <v>0.16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="3">
+        <f>(1.23*5+G32)/6</f>
+        <v>1.0533333333333335</v>
+      </c>
+      <c r="H33" s="6">
+        <f>(0*5+H32)/6</f>
+        <v>18.3</v>
+      </c>
+      <c r="K33" t="s">
+        <v>119</v>
+      </c>
+      <c r="L33" s="6">
+        <f>(0*5+L32)/6</f>
+        <v>14587.5</v>
+      </c>
+      <c r="M33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>225</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D34" t="s">
+        <v>233</v>
+      </c>
+      <c r="E34">
+        <v>0.13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>229</v>
+      </c>
+      <c r="G34" s="4">
+        <f>(0.25*5+G32)/6</f>
+        <v>0.23666666666666666</v>
+      </c>
+      <c r="H34" s="6">
+        <f>(H77*5+H32)/6</f>
+        <v>25.645</v>
+      </c>
+      <c r="K34" t="s">
+        <v>229</v>
+      </c>
+      <c r="L34" s="6">
+        <f>(L77*5+L32)/6</f>
+        <v>25572.5</v>
+      </c>
+      <c r="M34">
+        <v>60</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>59</v>
+        <v>226</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>234</v>
       </c>
       <c r="E35">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
       <c r="F35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G35">
-        <v>0.19</v>
-      </c>
-      <c r="H35">
-        <v>71</v>
-      </c>
-      <c r="I35">
-        <v>196</v>
+        <v>118</v>
+      </c>
+      <c r="G35" s="4">
+        <f>(0.25*5+G32)/6</f>
+        <v>0.23666666666666666</v>
+      </c>
+      <c r="H35" s="6">
+        <f>(H86*5+H32)/6</f>
+        <v>69.35208333333334</v>
       </c>
       <c r="K35" t="s">
-        <v>7</v>
+        <v>118</v>
+      </c>
+      <c r="L35" s="6">
+        <f>(L86*5+L32)/6</f>
+        <v>52612.5</v>
       </c>
       <c r="M35">
         <v>60</v>
       </c>
-      <c r="N35" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36">
-        <v>0.24</v>
-      </c>
-      <c r="F36" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36">
-        <v>0.13</v>
-      </c>
-      <c r="H36">
-        <v>74</v>
-      </c>
-      <c r="I36">
-        <v>225</v>
-      </c>
-      <c r="K36" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36">
-        <v>60</v>
-      </c>
-      <c r="N36" t="s">
-        <v>64</v>
-      </c>
+      <c r="C36" s="9"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="6"/>
+      <c r="L36" s="6"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F37" t="s">
-        <v>63</v>
-      </c>
-      <c r="G37">
-        <v>0.11</v>
-      </c>
-      <c r="H37">
-        <v>76</v>
-      </c>
-      <c r="I37">
-        <v>239</v>
-      </c>
-      <c r="K37" t="s">
-        <v>7</v>
-      </c>
-      <c r="M37">
-        <v>60</v>
-      </c>
-      <c r="N37" t="s">
-        <v>64</v>
-      </c>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="E38">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F38" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="G38">
-        <v>0.25</v>
-      </c>
-      <c r="H38">
-        <v>-22</v>
+        <v>0.19</v>
+      </c>
+      <c r="H38" s="6">
+        <v>71</v>
       </c>
       <c r="I38">
-        <v>68</v>
+        <v>196</v>
       </c>
       <c r="K38" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="M38">
         <v>60</v>
@@ -5204,31 +5387,31 @@
         <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="E39">
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="F39" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="G39">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H39">
-        <v>-26</v>
+        <v>0.13</v>
+      </c>
+      <c r="H39" s="6">
+        <v>74</v>
       </c>
       <c r="I39">
-        <v>87</v>
+        <v>225</v>
       </c>
       <c r="K39" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="M39">
         <v>60</v>
@@ -5242,36 +5425,74 @@
         <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="D40" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="E40">
-        <v>0.32</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F40" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="G40">
-        <v>0.12</v>
-      </c>
-      <c r="H40">
-        <v>-27</v>
+        <v>0.11</v>
+      </c>
+      <c r="H40" s="6">
+        <v>76</v>
       </c>
       <c r="I40">
-        <v>89</v>
+        <v>239</v>
       </c>
       <c r="K40" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="M40">
         <v>60</v>
       </c>
       <c r="N40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41">
+        <v>0.15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41">
+        <v>0.25</v>
+      </c>
+      <c r="H41" s="6">
+        <v>-22</v>
+      </c>
+      <c r="I41">
+        <v>68</v>
+      </c>
+      <c r="K41" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41">
+        <v>60</v>
+      </c>
+      <c r="N41" t="s">
         <v>64</v>
       </c>
     </row>
@@ -5280,37 +5501,37 @@
         <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D42" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="E42">
-        <v>0.16</v>
+        <v>0.3</v>
       </c>
       <c r="F42" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="G42">
-        <v>0.16</v>
-      </c>
-      <c r="H42">
-        <v>158.6</v>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H42" s="6">
+        <v>-26</v>
+      </c>
+      <c r="I42">
+        <v>87</v>
       </c>
       <c r="K42" t="s">
-        <v>7</v>
-      </c>
-      <c r="L42">
-        <v>181139</v>
+        <v>16</v>
       </c>
       <c r="M42">
         <v>60</v>
       </c>
       <c r="N42" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
@@ -5318,155 +5539,116 @@
         <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="E43">
         <v>0.32</v>
       </c>
       <c r="F43" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="G43">
-        <v>0.1</v>
-      </c>
-      <c r="H43">
-        <v>186.8</v>
+        <v>0.12</v>
+      </c>
+      <c r="H43" s="6">
+        <v>-27</v>
+      </c>
+      <c r="I43">
+        <v>89</v>
       </c>
       <c r="K43" t="s">
-        <v>7</v>
-      </c>
-      <c r="L43">
-        <v>210730</v>
+        <v>16</v>
       </c>
       <c r="M43">
         <v>60</v>
       </c>
       <c r="N43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" t="s">
-        <v>133</v>
-      </c>
-      <c r="E44" s="3">
-        <f>250*E42/(250+460)+460*E43/(250+460)</f>
-        <v>0.26366197183098594</v>
-      </c>
-      <c r="F44" t="s">
-        <v>141</v>
-      </c>
-      <c r="G44" s="3">
-        <f>250*G42/(250+460)+460*G43/(250+460)</f>
-        <v>0.12112676056338029</v>
-      </c>
-      <c r="H44" s="3">
-        <f>250*H42/(250+460)+460*H43/(250+460)</f>
-        <v>176.87042253521128</v>
-      </c>
-      <c r="K44" t="s">
-        <v>7</v>
-      </c>
-      <c r="L44" s="6">
-        <f>250*L42/(250+460)+460*L43/(250+460)</f>
-        <v>200310.63380281688</v>
-      </c>
-      <c r="M44">
-        <v>60</v>
-      </c>
-      <c r="N44" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>164</v>
+      <c r="B45" t="s">
+        <v>135</v>
       </c>
       <c r="C45" t="s">
         <v>116</v>
       </c>
       <c r="D45" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="E45">
         <v>0.16</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G45" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="H45" s="3">
-        <v>160.6</v>
+      <c r="F45" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45">
+        <v>0.16</v>
+      </c>
+      <c r="H45" s="6">
+        <v>158.6</v>
       </c>
       <c r="K45" t="s">
         <v>7</v>
       </c>
-      <c r="L45" s="6">
-        <v>196764</v>
+      <c r="L45">
+        <v>181139</v>
       </c>
       <c r="M45">
         <v>60</v>
       </c>
       <c r="N45" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>165</v>
+      <c r="B46" t="s">
+        <v>136</v>
       </c>
       <c r="C46" t="s">
         <v>116</v>
       </c>
       <c r="D46" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="E46">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G46" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="H46" s="3">
-        <v>178.5</v>
+        <v>0.32</v>
+      </c>
+      <c r="F46" t="s">
+        <v>141</v>
+      </c>
+      <c r="G46">
+        <v>0.1</v>
+      </c>
+      <c r="H46" s="6">
+        <v>186.8</v>
       </c>
       <c r="K46" t="s">
         <v>7</v>
       </c>
-      <c r="L46" s="6">
-        <v>363719</v>
+      <c r="L46">
+        <v>210730</v>
       </c>
       <c r="M46">
         <v>60</v>
       </c>
       <c r="N46" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -5474,155 +5656,203 @@
         <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="D47" t="s">
-        <v>160</v>
-      </c>
-      <c r="E47" s="4">
-        <f>126.7*E45/(126.7+140)+140*E46/(126.7+140)</f>
-        <v>0.14950131233595804</v>
+        <v>133</v>
+      </c>
+      <c r="E47" s="3">
+        <f>250*E45/(250+460)+460*E46/(250+460)</f>
+        <v>0.26366197183098594</v>
       </c>
       <c r="F47" t="s">
-        <v>169</v>
-      </c>
-      <c r="G47" s="8">
-        <f>126.7*G45/(126.7+140)+140*G46/(126.7+140)</f>
-        <v>0.16149606299212599</v>
+        <v>141</v>
+      </c>
+      <c r="G47" s="3">
+        <f>250*G45/(250+460)+460*G46/(250+460)</f>
+        <v>0.12112676056338029</v>
       </c>
       <c r="H47" s="6">
-        <f>126.7*H45/(126.7+140)+140*H46/(126.7+140)</f>
-        <v>169.99632545931757</v>
+        <f>250*H45/(250+460)+460*H46/(250+460)</f>
+        <v>176.87042253521128</v>
       </c>
       <c r="K47" t="s">
         <v>7</v>
       </c>
       <c r="L47" s="6">
-        <f>126.7*L45/(126.7+140)+140*L46/(126.7+140)</f>
-        <v>284404.41994750657</v>
+        <f>250*L45/(250+460)+460*L46/(250+460)</f>
+        <v>200310.63380281688</v>
       </c>
       <c r="M47">
         <v>60</v>
       </c>
       <c r="N47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
+        <v>221</v>
+      </c>
+      <c r="C48" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48">
+        <v>0.16</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="H48" s="6">
+        <v>160.6</v>
+      </c>
+      <c r="K48" t="s">
+        <v>7</v>
+      </c>
+      <c r="L48" s="6">
+        <v>196764</v>
+      </c>
+      <c r="M48">
+        <v>60</v>
+      </c>
+      <c r="N48" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" t="s">
+        <v>222</v>
+      </c>
+      <c r="C49" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="H49" s="6">
+        <v>178.5</v>
+      </c>
+      <c r="K49" t="s">
+        <v>7</v>
+      </c>
+      <c r="L49" s="6">
+        <v>363719</v>
+      </c>
+      <c r="M49">
+        <v>60</v>
+      </c>
+      <c r="N49" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
-        <v>106</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
+        <v>160</v>
+      </c>
+      <c r="E50" s="4">
+        <f>126.7*E48/(126.7+140)+140*E49/(126.7+140)</f>
+        <v>0.14950131233595804</v>
       </c>
       <c r="F50" t="s">
-        <v>98</v>
-      </c>
-      <c r="G50" t="s">
-        <v>98</v>
-      </c>
-      <c r="H50">
-        <v>58</v>
-      </c>
-      <c r="I50">
-        <v>126</v>
+        <v>169</v>
+      </c>
+      <c r="G50" s="7">
+        <f>126.7*G48/(126.7+140)+140*G49/(126.7+140)</f>
+        <v>0.16149606299212599</v>
+      </c>
+      <c r="H50" s="6">
+        <f>126.7*H48/(126.7+140)+140*H49/(126.7+140)</f>
+        <v>169.99632545931757</v>
       </c>
       <c r="K50" t="s">
         <v>7</v>
       </c>
+      <c r="L50" s="6">
+        <f>126.7*L48/(126.7+140)+140*L49/(126.7+140)</f>
+        <v>284404.41994750657</v>
+      </c>
       <c r="M50">
         <v>60</v>
       </c>
       <c r="N50" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" t="s">
-        <v>110</v>
-      </c>
-      <c r="C51" t="s">
-        <v>111</v>
-      </c>
-      <c r="D51" t="s">
-        <v>107</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51" t="s">
-        <v>98</v>
-      </c>
-      <c r="G51" t="s">
-        <v>98</v>
-      </c>
-      <c r="H51">
-        <v>-55</v>
-      </c>
-      <c r="I51">
-        <v>39</v>
-      </c>
-      <c r="K51" t="s">
-        <v>16</v>
-      </c>
-      <c r="M51">
-        <v>60</v>
-      </c>
-      <c r="N51" t="s">
-        <v>112</v>
-      </c>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="D53" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="E53">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>142</v>
-      </c>
-      <c r="G53">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="H53">
-        <v>117.1</v>
+        <v>98</v>
+      </c>
+      <c r="G53" t="s">
+        <v>98</v>
+      </c>
+      <c r="H53" s="6">
+        <v>58</v>
+      </c>
+      <c r="I53">
+        <v>126</v>
       </c>
       <c r="K53" t="s">
         <v>7</v>
       </c>
-      <c r="L53">
-        <v>152763</v>
-      </c>
       <c r="M53">
         <v>60</v>
       </c>
       <c r="N53" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
@@ -5630,314 +5860,286 @@
         <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="E54">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>142</v>
-      </c>
-      <c r="G54">
-        <v>0.16</v>
-      </c>
-      <c r="H54">
-        <v>162.80000000000001</v>
+        <v>98</v>
+      </c>
+      <c r="G54" t="s">
+        <v>98</v>
+      </c>
+      <c r="H54" s="6">
+        <v>-55</v>
+      </c>
+      <c r="I54">
+        <v>39</v>
       </c>
       <c r="K54" t="s">
-        <v>7</v>
-      </c>
-      <c r="L54">
-        <v>206295</v>
+        <v>16</v>
       </c>
       <c r="M54">
         <v>60</v>
       </c>
       <c r="N54" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>96</v>
-      </c>
-      <c r="B55" t="s">
-        <v>131</v>
-      </c>
-      <c r="C55" t="s">
-        <v>138</v>
-      </c>
-      <c r="D55" t="s">
-        <v>130</v>
-      </c>
-      <c r="E55" s="5">
-        <f>387*E53/(387+242)+242*E54/(387+242)</f>
-        <v>0.3</v>
-      </c>
-      <c r="F55" t="s">
-        <v>142</v>
-      </c>
-      <c r="G55" s="4">
-        <f>387*G53/(387+242)+242*G54/(387+242)</f>
-        <v>0.23383147853736092</v>
-      </c>
-      <c r="H55" s="3">
-        <f>387*H53/(387+242)+242*H54/(387+242)</f>
-        <v>134.68251192368839</v>
-      </c>
-      <c r="K55" t="s">
-        <v>7</v>
-      </c>
-      <c r="L55" s="6">
-        <f>387*L53/(387+242)+242*L54/(387+242)</f>
-        <v>173358.7774244833</v>
-      </c>
-      <c r="M55" s="6">
-        <f>387*M53/(387+242)+242*M54/(387+242)</f>
-        <v>60</v>
-      </c>
-      <c r="N55" t="s">
-        <v>125</v>
-      </c>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C56" t="s">
-        <v>175</v>
+        <v>116</v>
       </c>
       <c r="D56" t="s">
-        <v>159</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>98</v>
+        <v>128</v>
+      </c>
+      <c r="E56">
+        <v>0.3</v>
       </c>
       <c r="F56" t="s">
-        <v>98</v>
-      </c>
-      <c r="G56" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="H56" s="3">
-        <v>105.6</v>
+        <v>142</v>
+      </c>
+      <c r="G56">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H56" s="6">
+        <v>117.1</v>
       </c>
       <c r="K56" t="s">
         <v>7</v>
       </c>
-      <c r="L56" s="6">
-        <v>143901</v>
-      </c>
-      <c r="M56" s="6">
+      <c r="L56">
+        <v>152763</v>
+      </c>
+      <c r="M56">
         <v>60</v>
       </c>
       <c r="N56" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
       <c r="C57" t="s">
-        <v>176</v>
+        <v>116</v>
       </c>
       <c r="D57" t="s">
-        <v>174</v>
-      </c>
-      <c r="E57" s="4">
-        <v>0.03</v>
+        <v>129</v>
+      </c>
+      <c r="E57">
+        <v>0.3</v>
       </c>
       <c r="F57" t="s">
-        <v>63</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H57" s="3">
-        <v>114.4</v>
+        <v>142</v>
+      </c>
+      <c r="G57">
+        <v>0.16</v>
+      </c>
+      <c r="H57" s="6">
+        <v>162.80000000000001</v>
       </c>
       <c r="K57" t="s">
         <v>7</v>
       </c>
-      <c r="L57" s="6">
-        <v>154647</v>
-      </c>
-      <c r="M57" s="6">
+      <c r="L57">
+        <v>206295</v>
+      </c>
+      <c r="M57">
         <v>60</v>
       </c>
       <c r="N57" t="s">
-        <v>170</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" t="s">
+        <v>130</v>
+      </c>
+      <c r="E58" s="5">
+        <f>387*E56/(387+242)+242*E57/(387+242)</f>
+        <v>0.3</v>
+      </c>
+      <c r="F58" t="s">
+        <v>142</v>
+      </c>
+      <c r="G58" s="4">
+        <f>387*G56/(387+242)+242*G57/(387+242)</f>
+        <v>0.23383147853736092</v>
+      </c>
+      <c r="H58" s="6">
+        <f>387*H56/(387+242)+242*H57/(387+242)</f>
+        <v>134.68251192368839</v>
+      </c>
+      <c r="K58" t="s">
+        <v>7</v>
+      </c>
+      <c r="L58" s="6">
+        <f>387*L56/(387+242)+242*L57/(387+242)</f>
+        <v>173358.7774244833</v>
+      </c>
+      <c r="M58" s="6">
+        <f>387*M56/(387+242)+242*M57/(387+242)</f>
+        <v>60</v>
+      </c>
+      <c r="N58" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="D59" t="s">
-        <v>37</v>
+        <v>159</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="F59" t="s">
-        <v>38</v>
-      </c>
-      <c r="G59" t="s">
-        <v>40</v>
-      </c>
-      <c r="H59">
-        <f>249/1.6/1.5</f>
-        <v>103.75</v>
-      </c>
-      <c r="I59">
-        <f>1170/1.6/1.5*3600/1000</f>
-        <v>1755</v>
+        <v>98</v>
+      </c>
+      <c r="G59" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="H59" s="6">
+        <v>105.6</v>
       </c>
       <c r="K59" t="s">
-        <v>46</v>
-      </c>
-      <c r="L59">
-        <f>333000/1.6/1.5</f>
-        <v>138750</v>
-      </c>
-      <c r="M59">
-        <v>30</v>
-      </c>
-      <c r="N59" s="2" t="s">
-        <v>41</v>
+        <v>7</v>
+      </c>
+      <c r="L59" s="6">
+        <v>143901</v>
+      </c>
+      <c r="M59" s="6">
+        <v>60</v>
+      </c>
+      <c r="N59" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>173</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>172</v>
       </c>
       <c r="C60" t="s">
-        <v>43</v>
+        <v>176</v>
       </c>
       <c r="D60" t="s">
-        <v>48</v>
+        <v>174</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0.03</v>
       </c>
       <c r="F60" t="s">
-        <v>47</v>
-      </c>
-      <c r="G60" t="s">
-        <v>44</v>
-      </c>
-      <c r="H60" s="4">
-        <f>392/1.5/1.6</f>
-        <v>163.33333333333331</v>
-      </c>
-      <c r="I60">
-        <f>1740/1.6/1.5*3600/1000</f>
-        <v>2610</v>
+        <v>63</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H60" s="6">
+        <v>114.4</v>
       </c>
       <c r="K60" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="L60" s="6">
-        <f>440000/1.5/1.6</f>
-        <v>183333.33333333331</v>
-      </c>
-      <c r="M60">
-        <v>30</v>
+        <v>154647</v>
+      </c>
+      <c r="M60" s="6">
+        <v>60</v>
       </c>
       <c r="N60" t="s">
-        <v>41</v>
-      </c>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>36</v>
-      </c>
-      <c r="B62" t="s">
-        <v>75</v>
-      </c>
-      <c r="C62" t="s">
-        <v>78</v>
-      </c>
-      <c r="D62" t="s">
-        <v>86</v>
-      </c>
-      <c r="F62" t="s">
-        <v>47</v>
-      </c>
-      <c r="G62">
-        <v>1.3</v>
-      </c>
-      <c r="H62">
-        <v>206</v>
-      </c>
-      <c r="I62">
-        <v>1150</v>
-      </c>
-      <c r="K62" t="s">
-        <v>80</v>
-      </c>
-      <c r="L62">
-        <v>307000</v>
-      </c>
-      <c r="M62">
-        <v>30</v>
-      </c>
-      <c r="N62" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="H62" s="6"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>36</v>
       </c>
       <c r="B63" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="D63" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="F63" t="s">
-        <v>82</v>
-      </c>
-      <c r="G63">
-        <v>0.9</v>
-      </c>
-      <c r="H63">
-        <v>272</v>
+        <v>38</v>
+      </c>
+      <c r="G63" t="s">
+        <v>40</v>
+      </c>
+      <c r="H63" s="6">
+        <f>249/1.6/1.5</f>
+        <v>103.75</v>
       </c>
       <c r="I63">
-        <v>1520</v>
+        <f>1170/1.6/1.5*3600/1000</f>
+        <v>1755</v>
       </c>
       <c r="K63" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="L63">
-        <v>399000</v>
+        <f>333000/1.6/1.5</f>
+        <v>138750</v>
       </c>
       <c r="M63">
         <v>30</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -5945,74 +6147,81 @@
         <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C64" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="D64" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="F64" t="s">
-        <v>83</v>
-      </c>
-      <c r="G64">
-        <v>0.74</v>
-      </c>
-      <c r="H64">
-        <v>287</v>
+        <v>47</v>
+      </c>
+      <c r="G64" t="s">
+        <v>44</v>
+      </c>
+      <c r="H64" s="6">
+        <f>392/1.5/1.6</f>
+        <v>163.33333333333331</v>
       </c>
       <c r="I64">
-        <v>1630</v>
+        <f>1740/1.6/1.5*3600/1000</f>
+        <v>2610</v>
       </c>
       <c r="K64" t="s">
-        <v>80</v>
-      </c>
-      <c r="L64">
-        <v>422000</v>
+        <v>45</v>
+      </c>
+      <c r="L64" s="6">
+        <f>440000/1.5/1.6</f>
+        <v>183333.33333333331</v>
       </c>
       <c r="M64">
         <v>30</v>
       </c>
-      <c r="N64" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="N64" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H65" s="6"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="D66" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
       <c r="F66" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G66">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="H66" s="6">
-        <f>276/1.75/1.3</f>
-        <v>121.31868131868131</v>
+        <v>206</v>
+      </c>
+      <c r="I66">
+        <v>1150</v>
       </c>
       <c r="K66" t="s">
-        <v>148</v>
-      </c>
-      <c r="L66" s="6">
-        <f>352000/1.75/1.3</f>
-        <v>154725.27472527471</v>
+        <v>80</v>
+      </c>
+      <c r="L66">
+        <v>307000</v>
       </c>
       <c r="M66">
         <v>30</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>149</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -6020,36 +6229,37 @@
         <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>150</v>
+        <v>76</v>
       </c>
       <c r="C67" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="D67" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
       <c r="F67" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="G67">
-        <v>1.23</v>
-      </c>
-      <c r="H67" s="6">
-        <f>220/1.75/1.3</f>
-        <v>96.703296703296701</v>
+        <v>0.9</v>
+      </c>
+      <c r="H67">
+        <v>272</v>
+      </c>
+      <c r="I67">
+        <v>1520</v>
       </c>
       <c r="K67" t="s">
-        <v>148</v>
-      </c>
-      <c r="L67" s="6">
-        <f>291000/1.75/1.3</f>
-        <v>127912.08791208791</v>
+        <v>80</v>
+      </c>
+      <c r="L67">
+        <v>399000</v>
       </c>
       <c r="M67">
         <v>30</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>149</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -6057,80 +6267,977 @@
         <v>36</v>
       </c>
       <c r="B68" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="D68" t="s">
-        <v>155</v>
-      </c>
-      <c r="G68" s="4">
-        <f>393*G66/(393+58)+58*G67/(393+58)</f>
-        <v>0.94243902439024385</v>
-      </c>
-      <c r="H68" s="6">
-        <f>393*H66/(393+58)+58*H67/(393+58)</f>
-        <v>118.15306644574936</v>
+        <v>88</v>
+      </c>
+      <c r="F68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G68">
+        <v>0.74</v>
+      </c>
+      <c r="H68">
+        <v>287</v>
+      </c>
+      <c r="I68">
+        <v>1630</v>
       </c>
       <c r="K68" t="s">
-        <v>148</v>
-      </c>
-      <c r="L68" s="6">
-        <f>393*L66/(393+58)+58*L67/(393+58)</f>
-        <v>151277.01566725958</v>
+        <v>80</v>
+      </c>
+      <c r="L68">
+        <v>422000</v>
       </c>
       <c r="M68">
         <v>30</v>
       </c>
-      <c r="N68" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="N68" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>36</v>
       </c>
-      <c r="B69" t="s">
-        <v>161</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B70" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70" t="s">
+        <v>146</v>
+      </c>
+      <c r="D70" t="s">
+        <v>147</v>
+      </c>
+      <c r="F70" t="s">
+        <v>38</v>
+      </c>
+      <c r="G70">
+        <v>0.9</v>
+      </c>
+      <c r="H70" s="6">
+        <f>276/1.75/1.3</f>
+        <v>121.31868131868131</v>
+      </c>
+      <c r="K70" t="s">
+        <v>148</v>
+      </c>
+      <c r="L70" s="6">
+        <f>352000/1.75/1.3</f>
+        <v>154725.27472527471</v>
+      </c>
+      <c r="M70">
+        <v>30</v>
+      </c>
+      <c r="N70" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" t="s">
+        <v>150</v>
+      </c>
+      <c r="C71" t="s">
         <v>151</v>
       </c>
-      <c r="D69" t="s">
-        <v>158</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="D71" t="s">
+        <v>152</v>
+      </c>
+      <c r="F71" t="s">
         <v>47</v>
       </c>
-      <c r="G69">
-        <v>1.3</v>
-      </c>
-      <c r="H69" s="6">
+      <c r="G71">
+        <v>1.23</v>
+      </c>
+      <c r="H71" s="6">
         <f>220/1.75/1.3</f>
         <v>96.703296703296701</v>
       </c>
-      <c r="K69" t="s">
+      <c r="K71" t="s">
         <v>148</v>
       </c>
-      <c r="L69" s="6">
+      <c r="L71" s="6">
         <f>291000/1.75/1.3</f>
         <v>127912.08791208791</v>
       </c>
-      <c r="M69">
+      <c r="M71">
         <v>30</v>
       </c>
-      <c r="N69" s="2" t="s">
+      <c r="N71" s="2" t="s">
         <v>149</v>
       </c>
     </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D72" t="s">
+        <v>155</v>
+      </c>
+      <c r="G72" s="4">
+        <f>393*G70/(393+58)+58*G71/(393+58)</f>
+        <v>0.94243902439024385</v>
+      </c>
+      <c r="H72" s="6">
+        <f>393*H70/(393+58)+58*H71/(393+58)</f>
+        <v>118.15306644574936</v>
+      </c>
+      <c r="K72" t="s">
+        <v>148</v>
+      </c>
+      <c r="L72" s="6">
+        <f>393*L70/(393+58)+58*L71/(393+58)</f>
+        <v>151277.01566725958</v>
+      </c>
+      <c r="M72">
+        <v>30</v>
+      </c>
+      <c r="N72" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" t="s">
+        <v>161</v>
+      </c>
+      <c r="C73" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73" t="s">
+        <v>158</v>
+      </c>
+      <c r="F73" t="s">
+        <v>47</v>
+      </c>
+      <c r="G73">
+        <v>1.3</v>
+      </c>
+      <c r="H73" s="6">
+        <f>220/1.75/1.3</f>
+        <v>96.703296703296701</v>
+      </c>
+      <c r="K73" t="s">
+        <v>148</v>
+      </c>
+      <c r="L73" s="6">
+        <f>291000/1.75/1.3</f>
+        <v>127912.08791208791</v>
+      </c>
+      <c r="M73">
+        <v>30</v>
+      </c>
+      <c r="N73" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" t="s">
+        <v>230</v>
+      </c>
+      <c r="C74" t="s">
+        <v>231</v>
+      </c>
+      <c r="D74" t="s">
+        <v>235</v>
+      </c>
+      <c r="G74" s="3">
+        <f>(3.06*5+1)/6</f>
+        <v>2.7166666666666668</v>
+      </c>
+      <c r="H74" s="6">
+        <f>(0*5+256/(1.75*1.3))/6</f>
+        <v>18.754578754578755</v>
+      </c>
+      <c r="L74" s="6">
+        <f>(0*5+335000/(1.75*1.3))/6</f>
+        <v>24542.124542124544</v>
+      </c>
+      <c r="M74">
+        <v>30</v>
+      </c>
+      <c r="N74" s="2"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="N75" s="2"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="N76" s="2"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" t="s">
+        <v>197</v>
+      </c>
+      <c r="C77" t="s">
+        <v>198</v>
+      </c>
+      <c r="D77" t="s">
+        <v>197</v>
+      </c>
+      <c r="E77">
+        <v>0.13</v>
+      </c>
+      <c r="F77" t="s">
+        <v>15</v>
+      </c>
+      <c r="G77">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H77" s="6">
+        <f>1.13*AVERAGE(20,100)*E77</f>
+        <v>8.8140000000000001</v>
+      </c>
+      <c r="K77" t="s">
+        <v>15</v>
+      </c>
+      <c r="L77" s="1">
+        <f>1690*AVERAGE(20,100)*E77</f>
+        <v>13182</v>
+      </c>
+      <c r="M77">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>179</v>
+      </c>
+      <c r="B78" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" t="s">
+        <v>199</v>
+      </c>
+      <c r="D78" t="s">
+        <v>180</v>
+      </c>
+      <c r="E78">
+        <v>0.18</v>
+      </c>
+      <c r="F78" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H78" s="6">
+        <f>1.13*AVERAGE(20,100)*E78</f>
+        <v>12.203999999999999</v>
+      </c>
+      <c r="K78" t="s">
+        <v>15</v>
+      </c>
+      <c r="L78" s="1">
+        <f t="shared" ref="L78" si="1">1690*AVERAGE(20,100)*E78</f>
+        <v>18252</v>
+      </c>
+      <c r="M78">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>179</v>
+      </c>
+      <c r="B79" t="s">
+        <v>213</v>
+      </c>
+      <c r="C79" t="s">
+        <v>214</v>
+      </c>
+      <c r="D79" t="s">
+        <v>213</v>
+      </c>
+      <c r="E79">
+        <v>0.08</v>
+      </c>
+      <c r="F79" t="s">
+        <v>15</v>
+      </c>
+      <c r="G79">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H79" s="6">
+        <f>1.13*AVERAGE(20,100)*E79</f>
+        <v>5.4239999999999995</v>
+      </c>
+      <c r="K79" t="s">
+        <v>15</v>
+      </c>
+      <c r="L79" s="1">
+        <f>1690*AVERAGE(20,100)*E79</f>
+        <v>8112</v>
+      </c>
+      <c r="M79">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>179</v>
+      </c>
+      <c r="B80" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80" t="s">
+        <v>200</v>
+      </c>
+      <c r="D80" t="s">
+        <v>181</v>
+      </c>
+      <c r="E80">
+        <v>0.13</v>
+      </c>
+      <c r="F80" t="s">
+        <v>9</v>
+      </c>
+      <c r="G80">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H80" s="6">
+        <f>1.13*AVERAGE(32,160)*E80</f>
+        <v>14.102399999999999</v>
+      </c>
+      <c r="K80" t="s">
+        <v>9</v>
+      </c>
+      <c r="L80" s="8">
+        <f>1140*AVERAGE(32,160)*E80</f>
+        <v>14227.2</v>
+      </c>
+      <c r="M80">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>179</v>
+      </c>
+      <c r="B81" t="s">
+        <v>182</v>
+      </c>
+      <c r="C81" t="s">
+        <v>201</v>
+      </c>
+      <c r="D81" t="s">
+        <v>182</v>
+      </c>
+      <c r="E81">
+        <v>0.18</v>
+      </c>
+      <c r="F81" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H81" s="6">
+        <f>1.13*AVERAGE(32,160)*E81</f>
+        <v>19.526399999999999</v>
+      </c>
+      <c r="K81" t="s">
+        <v>9</v>
+      </c>
+      <c r="L81" s="8">
+        <f>1140*AVERAGE(32,160)*E81</f>
+        <v>19699.2</v>
+      </c>
+      <c r="M81">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>179</v>
+      </c>
+      <c r="B82" t="s">
+        <v>215</v>
+      </c>
+      <c r="C82" t="s">
+        <v>216</v>
+      </c>
+      <c r="D82" t="s">
+        <v>215</v>
+      </c>
+      <c r="E82">
+        <v>0.08</v>
+      </c>
+      <c r="F82" t="s">
+        <v>9</v>
+      </c>
+      <c r="G82">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H82" s="6">
+        <f>1.13*AVERAGE(32,160)*E82</f>
+        <v>8.6783999999999999</v>
+      </c>
+      <c r="K82" t="s">
+        <v>9</v>
+      </c>
+      <c r="L82" s="8">
+        <f>1140*AVERAGE(32,160)*E82</f>
+        <v>8755.2000000000007</v>
+      </c>
+      <c r="M82">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>179</v>
+      </c>
+      <c r="B83" t="s">
+        <v>183</v>
+      </c>
+      <c r="C83" t="s">
+        <v>202</v>
+      </c>
+      <c r="D83" t="s">
+        <v>183</v>
+      </c>
+      <c r="E83">
+        <v>0.13</v>
+      </c>
+      <c r="F83" t="s">
+        <v>63</v>
+      </c>
+      <c r="G83">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H83" s="6">
+        <f>7.64*AVERAGE(15,40)*E83</f>
+        <v>27.312999999999999</v>
+      </c>
+      <c r="K83" t="s">
+        <v>63</v>
+      </c>
+      <c r="L83" s="8">
+        <f>5180*AVERAGE(15,40)*E83</f>
+        <v>18518.5</v>
+      </c>
+      <c r="M83">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>179</v>
+      </c>
+      <c r="B84" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" t="s">
+        <v>203</v>
+      </c>
+      <c r="D84" t="s">
+        <v>184</v>
+      </c>
+      <c r="E84">
+        <v>0.18</v>
+      </c>
+      <c r="F84" t="s">
+        <v>63</v>
+      </c>
+      <c r="G84">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H84" s="6">
+        <f>7.64*AVERAGE(15,40)*E84</f>
+        <v>37.817999999999998</v>
+      </c>
+      <c r="K84" t="s">
+        <v>63</v>
+      </c>
+      <c r="L84" s="8">
+        <f>5180*AVERAGE(15,40)*E84</f>
+        <v>25641</v>
+      </c>
+      <c r="M84">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>179</v>
+      </c>
+      <c r="B85" t="s">
+        <v>217</v>
+      </c>
+      <c r="C85" t="s">
+        <v>218</v>
+      </c>
+      <c r="D85" t="s">
+        <v>217</v>
+      </c>
+      <c r="E85">
+        <v>0.08</v>
+      </c>
+      <c r="F85" t="s">
+        <v>63</v>
+      </c>
+      <c r="G85">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H85" s="6">
+        <f>7.64*AVERAGE(15,40)*E85</f>
+        <v>16.808</v>
+      </c>
+      <c r="K85" t="s">
+        <v>63</v>
+      </c>
+      <c r="L85" s="8">
+        <f>5180*AVERAGE(15,40)*E85</f>
+        <v>11396</v>
+      </c>
+      <c r="M85">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>179</v>
+      </c>
+      <c r="B86" t="s">
+        <v>185</v>
+      </c>
+      <c r="C86" t="s">
+        <v>204</v>
+      </c>
+      <c r="D86" t="s">
+        <v>185</v>
+      </c>
+      <c r="E86">
+        <v>0.13</v>
+      </c>
+      <c r="F86" t="s">
+        <v>118</v>
+      </c>
+      <c r="G86">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H86" s="6">
+        <f>14.5*AVERAGE(30,35)*E86</f>
+        <v>61.262500000000003</v>
+      </c>
+      <c r="K86" t="s">
+        <v>118</v>
+      </c>
+      <c r="L86" s="1">
+        <f>10800*AVERAGE(30,35)*E86</f>
+        <v>45630</v>
+      </c>
+      <c r="M86">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>179</v>
+      </c>
+      <c r="B87" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" t="s">
+        <v>205</v>
+      </c>
+      <c r="D87" t="s">
+        <v>186</v>
+      </c>
+      <c r="E87">
+        <v>0.18</v>
+      </c>
+      <c r="F87" t="s">
+        <v>118</v>
+      </c>
+      <c r="G87">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H87" s="6">
+        <f>14.5*AVERAGE(30,35)*E87</f>
+        <v>84.825000000000003</v>
+      </c>
+      <c r="K87" t="s">
+        <v>118</v>
+      </c>
+      <c r="L87" s="1">
+        <f>10800*AVERAGE(30,35)*E87</f>
+        <v>63180</v>
+      </c>
+      <c r="M87">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" t="s">
+        <v>219</v>
+      </c>
+      <c r="C88" t="s">
+        <v>220</v>
+      </c>
+      <c r="D88" t="s">
+        <v>219</v>
+      </c>
+      <c r="E88">
+        <v>0.08</v>
+      </c>
+      <c r="F88" t="s">
+        <v>118</v>
+      </c>
+      <c r="G88">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H88" s="6">
+        <f>14.5*AVERAGE(30,35)*E88</f>
+        <v>37.700000000000003</v>
+      </c>
+      <c r="K88" t="s">
+        <v>118</v>
+      </c>
+      <c r="L88" s="1">
+        <f>10800*AVERAGE(30,35)*E88</f>
+        <v>28080</v>
+      </c>
+      <c r="M88">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>179</v>
+      </c>
+      <c r="B89" t="s">
+        <v>187</v>
+      </c>
+      <c r="C89" t="s">
+        <v>206</v>
+      </c>
+      <c r="D89" t="s">
+        <v>187</v>
+      </c>
+      <c r="E89">
+        <v>0.08</v>
+      </c>
+      <c r="F89" t="s">
+        <v>169</v>
+      </c>
+      <c r="G89">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H89" s="6">
+        <f>7.52*AVERAGE(30)*E89</f>
+        <v>18.047999999999998</v>
+      </c>
+      <c r="K89" t="s">
+        <v>169</v>
+      </c>
+      <c r="L89" s="1">
+        <f>6630*AVERAGE(30)*E89</f>
+        <v>15912</v>
+      </c>
+      <c r="M89">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>179</v>
+      </c>
+      <c r="B90" t="s">
+        <v>188</v>
+      </c>
+      <c r="C90" t="s">
+        <v>207</v>
+      </c>
+      <c r="D90" t="s">
+        <v>188</v>
+      </c>
+      <c r="E90">
+        <v>0.13</v>
+      </c>
+      <c r="F90" t="s">
+        <v>169</v>
+      </c>
+      <c r="G90">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H90" s="6">
+        <f>7.52*AVERAGE(30)*E90</f>
+        <v>29.327999999999999</v>
+      </c>
+      <c r="K90" t="s">
+        <v>169</v>
+      </c>
+      <c r="L90" s="1">
+        <f>6630*AVERAGE(30)*E90</f>
+        <v>25857</v>
+      </c>
+      <c r="M90">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" t="s">
+        <v>189</v>
+      </c>
+      <c r="C91" t="s">
+        <v>208</v>
+      </c>
+      <c r="D91" t="s">
+        <v>189</v>
+      </c>
+      <c r="E91">
+        <v>0.13</v>
+      </c>
+      <c r="F91" t="s">
+        <v>178</v>
+      </c>
+      <c r="G91">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H91" s="6">
+        <f>1.17*AVERAGE(100,165)*E91</f>
+        <v>20.153249999999996</v>
+      </c>
+      <c r="K91" t="s">
+        <v>178</v>
+      </c>
+      <c r="L91" s="1">
+        <f>1040*AVERAGE(100,165)*E91</f>
+        <v>17914</v>
+      </c>
+      <c r="M91">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>179</v>
+      </c>
+      <c r="B92" t="s">
+        <v>190</v>
+      </c>
+      <c r="C92" t="s">
+        <v>209</v>
+      </c>
+      <c r="D92" t="s">
+        <v>190</v>
+      </c>
+      <c r="E92">
+        <v>0.18</v>
+      </c>
+      <c r="F92" t="s">
+        <v>178</v>
+      </c>
+      <c r="G92">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H92" s="6">
+        <f>1.17*AVERAGE(100,165)*E92</f>
+        <v>27.904499999999995</v>
+      </c>
+      <c r="K92" t="s">
+        <v>178</v>
+      </c>
+      <c r="L92" s="1">
+        <f>1040*AVERAGE(100,165)*E92</f>
+        <v>24804</v>
+      </c>
+      <c r="M92">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>179</v>
+      </c>
+      <c r="B93" t="s">
+        <v>191</v>
+      </c>
+      <c r="C93" t="s">
+        <v>210</v>
+      </c>
+      <c r="D93" t="s">
+        <v>191</v>
+      </c>
+      <c r="E93">
+        <v>0.13</v>
+      </c>
+      <c r="F93" t="s">
+        <v>177</v>
+      </c>
+      <c r="G93">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H93" s="6">
+        <f>0.665*AVERAGE(148)*E93</f>
+        <v>12.794600000000001</v>
+      </c>
+      <c r="K93" t="s">
+        <v>177</v>
+      </c>
+      <c r="L93" s="8">
+        <f>860*AVERAGE(148)*E93</f>
+        <v>16546.400000000001</v>
+      </c>
+      <c r="M93">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>179</v>
+      </c>
+      <c r="B94" t="s">
+        <v>192</v>
+      </c>
+      <c r="C94" t="s">
+        <v>211</v>
+      </c>
+      <c r="D94" t="s">
+        <v>192</v>
+      </c>
+      <c r="E94">
+        <v>0.18</v>
+      </c>
+      <c r="F94" t="s">
+        <v>177</v>
+      </c>
+      <c r="G94">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H94" s="6">
+        <f>0.665*AVERAGE(148)*E94</f>
+        <v>17.715599999999998</v>
+      </c>
+      <c r="K94" t="s">
+        <v>177</v>
+      </c>
+      <c r="L94" s="8">
+        <f>860*AVERAGE(148)*E94</f>
+        <v>22910.399999999998</v>
+      </c>
+      <c r="M94">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>179</v>
+      </c>
+      <c r="B95" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" t="s">
+        <v>212</v>
+      </c>
+      <c r="D95" t="s">
+        <v>193</v>
+      </c>
+      <c r="F95" t="s">
+        <v>194</v>
+      </c>
+      <c r="G95">
+        <v>0.96</v>
+      </c>
+      <c r="H95" s="6">
+        <f>(257+17.1)/(1.75*1.3)</f>
+        <v>120.4835164835165</v>
+      </c>
+      <c r="L95" s="8">
+        <f>(335000+11060)/(1.75*1.3)</f>
+        <v>152114.28571428571</v>
+      </c>
+      <c r="M95">
+        <v>30</v>
+      </c>
+      <c r="N95" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L96" s="1"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>196</v>
+      </c>
+      <c r="C97" t="s">
+        <v>196</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N59" r:id="rId1" xr:uid="{61032813-A891-F145-949A-3FC78FBCD676}"/>
-    <hyperlink ref="N66" r:id="rId2" xr:uid="{9A37C0FD-BB04-014B-BFC0-4A028B31EFB5}"/>
-    <hyperlink ref="N67" r:id="rId3" xr:uid="{E7FC74C7-197C-9E4B-BF0B-5F1705E181B5}"/>
-    <hyperlink ref="N69" r:id="rId4" xr:uid="{470944A1-1EDF-7C46-BF0C-F1995000D973}"/>
+    <hyperlink ref="N63" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N70" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N71" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N73" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>